<commit_message>
MS ready for submission
</commit_message>
<xml_diff>
--- a/analysis/Edited Data.xlsx
+++ b/analysis/Edited Data.xlsx
@@ -1,23 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew\Documents\Papers and Projects\Curculio Mechanical Testing\Tensile Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew\Documents\GitHub\curculio-tensile\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0585F7AB-737E-47D7-A4E3-342DCECD9CE0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -131,7 +137,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -171,74 +177,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -250,577 +188,15 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Endocuticle surface</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> area and maximum tensile force</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>caryae</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$J$2:$J$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>2.319864263551772E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.6159472589648925E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.8862425186149497E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.5104067156076326E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$L$2:$L$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>5.3342738000000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6.4675808000000004</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.5840825999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.3216481</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D5C9-4A4B-B8D7-05607FBA62E0}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$6</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>humeralis</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$J$6:$J$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>1.7228359264590209E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.9139448218277205E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$L$6:$L$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>2.5828912000000002</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.2311338999999997</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-D5C9-4A4B-B8D7-05607FBA62E0}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$8</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>proboscideus</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$J$8:$J$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>1.0359068957651396E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.0839807557690123E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.4125851528106602E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$L$8:$L$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>2.1439984000000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.736783</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.1857110999999998</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-D5C9-4A4B-B8D7-05607FBA62E0}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$11</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>sulcatulus</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$J$11:$J$14</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>1.025208797090248E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.3353517657935155E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.7358573855385591E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.8015698268288752E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$L$11:$L$14</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>1.1852844</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.1271718000000002</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.4255108999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.6222240999999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-D5C9-4A4B-B8D7-05607FBA62E0}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$15</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>uniformis</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$J$15:$J$19</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1.3832904283183269E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.3364285575689791E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.6569269142881468E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.1185429240160192E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.1232759150574785E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$L$15:$L$19</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1.7587828999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.8501333</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.0222728000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.3878853000000002</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.4324250999999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-D5C9-4A4B-B8D7-05607FBA62E0}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$20</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>victoriensis</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$J$20</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>1.4040666402476294E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$L$20</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>2.1997905000000002</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-D5C9-4A4B-B8D7-05607FBA62E0}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="229241344"/>
-        <c:axId val="229237888"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="229241344"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Endocuticle</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> surface area (mm2)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="229237888"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="229237888"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>F max (N)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="229241344"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>371474</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>4761</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>742950</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="21" name="Chart 20" title="Endocuticle Area and Fmax">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="C0C0C0"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="000000"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1108,11 +484,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2011,34 +1387,34 @@
         <v>6.9123775000000008E-4</v>
       </c>
       <c r="I13">
-        <f>(E13-F13)*(H13^2)</f>
+        <f t="shared" ref="I13:I20" si="9">(E13-F13)*(H13^2)</f>
         <v>3.9918079699219127E-3</v>
       </c>
       <c r="J13">
-        <f>(F13-G13)*(H13^2)</f>
+        <f t="shared" ref="J13:J20" si="10">(F13-G13)*(H13^2)</f>
         <v>1.7358573855385591E-2</v>
       </c>
       <c r="K13">
-        <f>(E13-G13)*(H13^2)</f>
+        <f t="shared" ref="K13:K20" si="11">(E13-G13)*(H13^2)</f>
         <v>2.1350381825307505E-2</v>
       </c>
       <c r="L13">
         <v>2.4255108999999999</v>
       </c>
       <c r="M13">
-        <f>L13/K13</f>
+        <f t="shared" ref="M13:M20" si="12">L13/K13</f>
         <v>113.6050361930736</v>
       </c>
       <c r="N13">
-        <f>I13/K13</f>
+        <f t="shared" ref="N13:N20" si="13">I13/K13</f>
         <v>0.18696658460647553</v>
       </c>
       <c r="O13">
-        <f>J13/K13</f>
+        <f t="shared" ref="O13:O20" si="14">J13/K13</f>
         <v>0.81303341539352447</v>
       </c>
       <c r="P13">
-        <f>I13/J13</f>
+        <f t="shared" ref="P13:P20" si="15">I13/J13</f>
         <v>0.22996174704083958</v>
       </c>
       <c r="Q13">
@@ -2052,7 +1428,7 @@
         <v>1.8017985672943099E-6</v>
       </c>
       <c r="T13" s="2">
-        <f>Q13*S13*1000</f>
+        <f t="shared" ref="T13:T20" si="16">Q13*S13*1000</f>
         <v>5.0540449812605397</v>
       </c>
     </row>
@@ -2083,34 +1459,34 @@
         <v>6.9123775000000008E-4</v>
       </c>
       <c r="I14">
-        <f>(E14-F14)*(H14^2)</f>
+        <f t="shared" si="9"/>
         <v>4.2409336091661391E-3</v>
       </c>
       <c r="J14">
-        <f>(F14-G14)*(H14^2)</f>
+        <f t="shared" si="10"/>
         <v>1.8015698268288752E-2</v>
       </c>
       <c r="K14">
-        <f>(E14-G14)*(H14^2)</f>
+        <f t="shared" si="11"/>
         <v>2.2256631877454892E-2</v>
       </c>
       <c r="L14">
         <v>2.6222240999999999</v>
       </c>
       <c r="M14">
-        <f>L14/K14</f>
+        <f t="shared" si="12"/>
         <v>117.81765158528823</v>
       </c>
       <c r="N14">
-        <f>I14/K14</f>
+        <f t="shared" si="13"/>
         <v>0.19054696292398315</v>
       </c>
       <c r="O14">
-        <f>J14/K14</f>
+        <f t="shared" si="14"/>
         <v>0.80945303707601679</v>
       </c>
       <c r="P14">
-        <f>I14/J14</f>
+        <f t="shared" si="15"/>
         <v>0.23540212241626149</v>
       </c>
       <c r="Q14">
@@ -2124,7 +1500,7 @@
         <v>2.2849421347341202E-6</v>
       </c>
       <c r="T14" s="2">
-        <f>Q14*S14*1000</f>
+        <f t="shared" si="16"/>
         <v>5.1685391087685799</v>
       </c>
     </row>
@@ -2155,34 +1531,34 @@
         <v>1.8789271839718168E-3</v>
       </c>
       <c r="I15">
-        <f>(E15-F15)*(H15^2)</f>
+        <f t="shared" si="9"/>
         <v>4.0983858194847704E-3</v>
       </c>
       <c r="J15">
-        <f>(F15-G15)*(H15^2)</f>
+        <f t="shared" si="10"/>
         <v>1.3832904283183269E-2</v>
       </c>
       <c r="K15">
-        <f>(E15-G15)*(H15^2)</f>
+        <f t="shared" si="11"/>
         <v>1.7931290102668036E-2</v>
       </c>
       <c r="L15">
         <v>1.7587828999999999</v>
       </c>
       <c r="M15">
-        <f>L15/K15</f>
+        <f t="shared" si="12"/>
         <v>98.084571156333411</v>
       </c>
       <c r="N15">
-        <f>I15/K15</f>
+        <f t="shared" si="13"/>
         <v>0.22856056625144683</v>
       </c>
       <c r="O15">
-        <f>J15/K15</f>
+        <f t="shared" si="14"/>
         <v>0.77143943374855328</v>
       </c>
       <c r="P15">
-        <f>I15/J15</f>
+        <f t="shared" si="15"/>
         <v>0.29627804368365351</v>
       </c>
       <c r="Q15">
@@ -2196,7 +1572,7 @@
         <v>1.8017985672943099E-6</v>
       </c>
       <c r="T15" s="2">
-        <f>Q15*S15*1000</f>
+        <f t="shared" si="16"/>
         <v>4.5927845480331957</v>
       </c>
     </row>
@@ -2227,34 +1603,34 @@
         <v>6.9123775000000008E-4</v>
       </c>
       <c r="I16">
-        <f>(E16-F16)*(H16^2)</f>
+        <f t="shared" si="9"/>
         <v>3.3781666221261658E-3</v>
       </c>
       <c r="J16">
-        <f>(F16-G16)*(H16^2)</f>
+        <f t="shared" si="10"/>
         <v>1.3364285575689791E-2</v>
       </c>
       <c r="K16">
-        <f>(E16-G16)*(H16^2)</f>
+        <f t="shared" si="11"/>
         <v>1.6742452197815956E-2</v>
       </c>
       <c r="L16">
         <v>1.8501333</v>
       </c>
       <c r="M16">
-        <f>L16/K16</f>
+        <f t="shared" si="12"/>
         <v>110.5055148517222</v>
       </c>
       <c r="N16">
-        <f>I16/K16</f>
+        <f t="shared" si="13"/>
         <v>0.20177251111201297</v>
       </c>
       <c r="O16">
-        <f>J16/K16</f>
+        <f t="shared" si="14"/>
         <v>0.79822748888798711</v>
       </c>
       <c r="P16">
-        <f>I16/J16</f>
+        <f t="shared" si="15"/>
         <v>0.25277569855819271</v>
       </c>
       <c r="Q16">
@@ -2268,7 +1644,7 @@
         <v>1.43550512834468E-6</v>
       </c>
       <c r="T16" s="2">
-        <f>Q16*S16*1000</f>
+        <f t="shared" si="16"/>
         <v>4.4527499892677023</v>
       </c>
     </row>
@@ -2299,34 +1675,34 @@
         <v>6.9123775000000008E-4</v>
       </c>
       <c r="I17">
-        <f>(E17-F17)*(H17^2)</f>
+        <f t="shared" si="9"/>
         <v>3.8346052579632788E-3</v>
       </c>
       <c r="J17">
-        <f>(F17-G17)*(H17^2)</f>
+        <f t="shared" si="10"/>
         <v>1.6569269142881468E-2</v>
       </c>
       <c r="K17">
-        <f>(E17-G17)*(H17^2)</f>
+        <f t="shared" si="11"/>
         <v>2.0403874400844745E-2</v>
       </c>
       <c r="L17">
         <v>2.0222728000000001</v>
       </c>
       <c r="M17">
-        <f>L17/K17</f>
+        <f t="shared" si="12"/>
         <v>99.112196059993167</v>
       </c>
       <c r="N17">
-        <f>I17/K17</f>
+        <f t="shared" si="13"/>
         <v>0.18793515303174585</v>
       </c>
       <c r="O17">
-        <f>J17/K17</f>
+        <f t="shared" si="14"/>
         <v>0.81206484696825421</v>
       </c>
       <c r="P17">
-        <f>I17/J17</f>
+        <f t="shared" si="15"/>
         <v>0.23142875071292518</v>
       </c>
       <c r="Q17">
@@ -2340,7 +1716,7 @@
         <v>1.8017985672943099E-6</v>
       </c>
       <c r="T17" s="2">
-        <f>Q17*S17*1000</f>
+        <f t="shared" si="16"/>
         <v>5.4270172846904616</v>
       </c>
     </row>
@@ -2371,34 +1747,34 @@
         <v>6.9123775000000008E-4</v>
       </c>
       <c r="I18">
-        <f>(E18-F18)*(H18^2)</f>
+        <f t="shared" si="9"/>
         <v>3.3567578839776824E-3</v>
       </c>
       <c r="J18">
-        <f>(F18-G18)*(H18^2)</f>
+        <f t="shared" si="10"/>
         <v>1.1185429240160192E-2</v>
       </c>
       <c r="K18">
-        <f>(E18-G18)*(H18^2)</f>
+        <f t="shared" si="11"/>
         <v>1.4542187124137875E-2</v>
       </c>
       <c r="L18">
         <v>2.3878853000000002</v>
       </c>
       <c r="M18">
-        <f>L18/K18</f>
+        <f t="shared" si="12"/>
         <v>164.20400037601391</v>
       </c>
       <c r="N18">
-        <f>I18/K18</f>
+        <f t="shared" si="13"/>
         <v>0.23082895683593302</v>
       </c>
       <c r="O18">
-        <f>J18/K18</f>
+        <f t="shared" si="14"/>
         <v>0.76917104316406693</v>
       </c>
       <c r="P18">
-        <f>I18/J18</f>
+        <f t="shared" si="15"/>
         <v>0.30010094489048045</v>
       </c>
       <c r="Q18">
@@ -2412,7 +1788,7 @@
         <v>1.43550512834468E-6</v>
       </c>
       <c r="T18" s="2">
-        <f>Q18*S18*1000</f>
+        <f t="shared" si="16"/>
         <v>3.6863771695891381</v>
       </c>
     </row>
@@ -2443,34 +1819,34 @@
         <v>6.9123775000000008E-4</v>
       </c>
       <c r="I19">
-        <f>(E19-F19)*(H19^2)</f>
+        <f t="shared" si="9"/>
         <v>5.4446966036769571E-3</v>
       </c>
       <c r="J19">
-        <f>(F19-G19)*(H19^2)</f>
+        <f t="shared" si="10"/>
         <v>1.1232759150574785E-2</v>
       </c>
       <c r="K19">
-        <f>(E19-G19)*(H19^2)</f>
+        <f t="shared" si="11"/>
         <v>1.6677455754251742E-2</v>
       </c>
       <c r="L19">
         <v>1.4324250999999999</v>
       </c>
       <c r="M19">
-        <f>L19/K19</f>
+        <f t="shared" si="12"/>
         <v>85.889905577163248</v>
       </c>
       <c r="N19">
-        <f>I19/K19</f>
+        <f t="shared" si="13"/>
         <v>0.32647045711926947</v>
       </c>
       <c r="O19">
-        <f>J19/K19</f>
+        <f t="shared" si="14"/>
         <v>0.67352954288073064</v>
       </c>
       <c r="P19">
-        <f>I19/J19</f>
+        <f t="shared" si="15"/>
         <v>0.4847158681754829</v>
       </c>
       <c r="Q19">
@@ -2484,7 +1860,7 @@
         <v>1.43550512834468E-6</v>
       </c>
       <c r="T19" s="2">
-        <f>Q19*S19*1000</f>
+        <f t="shared" si="16"/>
         <v>4.0610440080870998</v>
       </c>
     </row>
@@ -2515,34 +1891,34 @@
         <v>1.8789271839718168E-3</v>
       </c>
       <c r="I20">
-        <f>(E20-F20)*(H20^2)</f>
+        <f t="shared" si="9"/>
         <v>1.0444570660249876E-2</v>
       </c>
       <c r="J20">
-        <f>(F20-G20)*(H20^2)</f>
+        <f t="shared" si="10"/>
         <v>1.4040666402476294E-2</v>
       </c>
       <c r="K20">
-        <f>(E20-G20)*(H20^2)</f>
+        <f t="shared" si="11"/>
         <v>2.4485237062726171E-2</v>
       </c>
       <c r="L20">
         <v>2.1997905000000002</v>
       </c>
       <c r="M20">
-        <f>L20/K20</f>
+        <f t="shared" si="12"/>
         <v>89.841503039753576</v>
       </c>
       <c r="N20">
-        <f>I20/K20</f>
+        <f t="shared" si="13"/>
         <v>0.42656604195797743</v>
       </c>
       <c r="O20">
-        <f>J20/K20</f>
+        <f t="shared" si="14"/>
         <v>0.57343395804202246</v>
       </c>
       <c r="P20">
-        <f>I20/J20</f>
+        <f t="shared" si="15"/>
         <v>0.74387998125272814</v>
       </c>
       <c r="Q20">
@@ -2556,7 +1932,7 @@
         <v>1.8017985672943099E-6</v>
       </c>
       <c r="T20" s="2">
-        <f>Q20*S20*1000</f>
+        <f t="shared" si="16"/>
         <v>5.3621525362678666</v>
       </c>
     </row>
@@ -2569,6 +1945,5 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>